<commit_message>
updating spreadsheet w/ HR/LR group stats
</commit_message>
<xml_diff>
--- a/Spreadsheets/PQBC_health_demos_stats.xlsx
+++ b/Spreadsheets/PQBC_health_demos_stats.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/madeleineseitz/Desktop/thesis/ABCD_Project/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F45EF8-BC9A-394E-9B02-67827031DA08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20BA855-69AC-A145-8C2B-3444DB093E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="780" windowWidth="33520" windowHeight="21360" xr2:uid="{61F63AC5-4840-6245-B940-56E6384DC10B}"/>
+    <workbookView xWindow="680" yWindow="780" windowWidth="33520" windowHeight="21360" activeTab="1" xr2:uid="{61F63AC5-4840-6245-B940-56E6384DC10B}"/>
   </bookViews>
   <sheets>
     <sheet name="Threshold 4" sheetId="3" r:id="rId1"/>
+    <sheet name="Matched HR and LR Groups" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="59">
   <si>
     <t>Test</t>
   </si>
@@ -189,6 +190,30 @@
   </si>
   <si>
     <t>(6465, 7)</t>
+  </si>
+  <si>
+    <t>Student's t-test</t>
+  </si>
+  <si>
+    <t>Statistical comparisons of demographics between HR and LR groups (HR defined as having endorsed 4+ PQ-BC items, LR having endorsed 0 PQ-BC items, having no history of family mental illness, and matched with HR on ethnicity, sex, and age)</t>
+  </si>
+  <si>
+    <t>(3226, 7)</t>
+  </si>
+  <si>
+    <t>(3226, 28)</t>
+  </si>
+  <si>
+    <t>(2012, 12)</t>
+  </si>
+  <si>
+    <t>(3226, 16)</t>
+  </si>
+  <si>
+    <t>(3226, 6)</t>
+  </si>
+  <si>
+    <t>(1984, 7)</t>
   </si>
 </sst>
 </file>
@@ -259,7 +284,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -306,12 +331,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -328,6 +366,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="1" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="1" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
@@ -645,7 +686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A673DAA3-215C-E04C-A5CD-D136D731029B}">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
@@ -1380,4 +1421,745 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{881785B7-7EBC-6A42-AE3B-30A3999191F8}">
+  <dimension ref="A1:K51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" customWidth="1"/>
+    <col min="8" max="8" width="22.5" customWidth="1"/>
+    <col min="9" max="10" width="23.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="5">
+        <v>4.4699999999999997E-2</v>
+      </c>
+      <c r="C7" s="7">
+        <v>105.3704</v>
+      </c>
+      <c r="D7" s="17">
+        <v>57.624299999999998</v>
+      </c>
+      <c r="E7" s="9">
+        <v>7.0998000000000001</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7">
+        <v>2</v>
+      </c>
+      <c r="D8" s="10">
+        <v>2</v>
+      </c>
+      <c r="E8" s="9">
+        <v>3</v>
+      </c>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0.83260000000000001</v>
+      </c>
+      <c r="C9" s="11">
+        <v>1.3155E-23</v>
+      </c>
+      <c r="D9" s="18">
+        <v>3.0692999999999999E-13</v>
+      </c>
+      <c r="E9" s="9">
+        <v>6.88E-2</v>
+      </c>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="7">
+        <v>24.469200000000001</v>
+      </c>
+      <c r="C14" s="7">
+        <v>23.581800000000001</v>
+      </c>
+      <c r="D14" s="7">
+        <v>7.4987000000000004</v>
+      </c>
+      <c r="E14" s="7">
+        <v>3.5390000000000001</v>
+      </c>
+      <c r="F14" s="7">
+        <v>14.6035</v>
+      </c>
+      <c r="G14" s="7">
+        <v>13.3368</v>
+      </c>
+      <c r="H14" s="7">
+        <v>20.963999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="11">
+        <v>1.9666000000000002E-121</v>
+      </c>
+      <c r="C15" s="11">
+        <v>1.4472E-113</v>
+      </c>
+      <c r="D15" s="11">
+        <v>8.2828000000000006E-14</v>
+      </c>
+      <c r="E15" s="7">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F15" s="11">
+        <v>8.1909000000000004E-47</v>
+      </c>
+      <c r="G15" s="11">
+        <v>1.5631000000000001E-39</v>
+      </c>
+      <c r="H15" s="11">
+        <v>1.4571E-91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="7">
+        <v>3224</v>
+      </c>
+      <c r="C16" s="7">
+        <v>3224</v>
+      </c>
+      <c r="D16" s="7">
+        <v>3224</v>
+      </c>
+      <c r="E16" s="7">
+        <v>3224</v>
+      </c>
+      <c r="F16" s="7">
+        <v>3211</v>
+      </c>
+      <c r="G16" s="7">
+        <v>3211</v>
+      </c>
+      <c r="H16" s="7">
+        <v>3211</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="7">
+        <v>12.9101</v>
+      </c>
+      <c r="C21" s="7">
+        <v>14.4697</v>
+      </c>
+      <c r="D21" s="7">
+        <v>11.6839</v>
+      </c>
+      <c r="E21" s="7">
+        <v>16.248799999999999</v>
+      </c>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="11">
+        <v>1.0868E-36</v>
+      </c>
+      <c r="C22" s="11">
+        <v>3.2460999999999998E-45</v>
+      </c>
+      <c r="D22" s="11">
+        <v>1.4623000000000001E-30</v>
+      </c>
+      <c r="E22" s="11">
+        <v>7.0683999999999997E-56</v>
+      </c>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="7">
+        <v>2010</v>
+      </c>
+      <c r="C23" s="7">
+        <v>2010</v>
+      </c>
+      <c r="D23" s="7">
+        <v>2010</v>
+      </c>
+      <c r="E23" s="7">
+        <v>2010</v>
+      </c>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="9"/>
+      <c r="B26" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="K26" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="7">
+        <v>9.4106000000000005</v>
+      </c>
+      <c r="C28" s="9">
+        <v>0.88429999999999997</v>
+      </c>
+      <c r="D28" s="9">
+        <v>-6.1199999999999997E-2</v>
+      </c>
+      <c r="E28" s="9">
+        <v>0.86429999999999996</v>
+      </c>
+      <c r="F28" s="9">
+        <v>-1.2743</v>
+      </c>
+      <c r="G28" s="9">
+        <v>1.85</v>
+      </c>
+      <c r="H28" s="9">
+        <v>0.79590000000000005</v>
+      </c>
+      <c r="I28" s="7">
+        <v>23.318200000000001</v>
+      </c>
+      <c r="J28" s="7">
+        <v>42.143000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="11">
+        <v>9.0816999999999996E-21</v>
+      </c>
+      <c r="C29" s="9">
+        <v>0.37659999999999999</v>
+      </c>
+      <c r="D29" s="9">
+        <v>0.95120000000000005</v>
+      </c>
+      <c r="E29" s="9">
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="F29" s="9">
+        <v>0.20269999999999999</v>
+      </c>
+      <c r="G29" s="9">
+        <v>6.4399999999999999E-2</v>
+      </c>
+      <c r="H29" s="9">
+        <v>0.37230000000000002</v>
+      </c>
+      <c r="I29" s="11">
+        <v>1E-4</v>
+      </c>
+      <c r="J29" s="11">
+        <v>1.5580999999999999E-8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="7">
+        <v>3224</v>
+      </c>
+      <c r="C30" s="9">
+        <v>2548</v>
+      </c>
+      <c r="D30" s="9">
+        <v>2548</v>
+      </c>
+      <c r="E30" s="9">
+        <v>2548</v>
+      </c>
+      <c r="F30" s="9">
+        <v>2548</v>
+      </c>
+      <c r="G30" s="9">
+        <v>2548</v>
+      </c>
+      <c r="H30" s="9">
+        <v>1</v>
+      </c>
+      <c r="I30" s="7">
+        <v>4</v>
+      </c>
+      <c r="J30" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="9"/>
+      <c r="B33" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="7">
+        <v>6.6585999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="11">
+        <v>3.2365000000000003E-11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="7">
+        <v>3224</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="9"/>
+      <c r="B40" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" s="7">
+        <v>7.1121999999999996</v>
+      </c>
+      <c r="C42" s="7">
+        <v>3.8546999999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="11">
+        <v>1.4002E-12</v>
+      </c>
+      <c r="C43" s="11">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" s="7">
+        <v>3224</v>
+      </c>
+      <c r="C44" s="7">
+        <v>3224</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="9"/>
+      <c r="B47" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D47" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" s="7">
+        <v>6.6764000000000001</v>
+      </c>
+      <c r="C49" s="7">
+        <v>4.5655000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="11">
+        <v>3.1689E-11</v>
+      </c>
+      <c r="C50" s="16">
+        <v>5.2884000000000001E-6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" s="7">
+        <v>1982</v>
+      </c>
+      <c r="C51" s="7">
+        <v>1982</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>